<commit_message>
add more conformer analysis stuff
</commit_message>
<xml_diff>
--- a/fragmented_approach/weighted/fragmented_approach_all_isomers_input_builder.xlsx
+++ b/fragmented_approach/weighted/fragmented_approach_all_isomers_input_builder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwb1j\OneDrive\Documents\GitHub\phosphine-ligands\fragmented_approach\weighted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1EF346-47C7-4857-8219-4793A72F60F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA41B0E3-0585-41B1-8068-621F06B3F28A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14427" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -782,13 +782,6 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="1"/>
@@ -830,6 +823,13 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -844,7 +844,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A3AC54E-9A9E-4EAC-9CD6-46941706A6B8}" name="Table4" displayName="Table4" ref="O1:P94" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5A3AC54E-9A9E-4EAC-9CD6-46941706A6B8}" name="Table4" displayName="Table4" ref="O1:P94" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="O1:P94" xr:uid="{E41C5667-10C2-42DB-A546-1C7EDA75AE73}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O2:P94">
     <sortCondition ref="O1:O94"/>
@@ -1145,7 +1145,7 @@
   <dimension ref="A1:CF59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -16219,7 +16219,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16232,7 +16232,7 @@
   <dimension ref="A1:U94"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:U1048576"/>
+      <selection activeCell="R73" sqref="R73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>